<commit_message>
add more information for table
</commit_message>
<xml_diff>
--- a/BangKeHoach-TLCN.xlsx
+++ b/BangKeHoach-TLCN.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>STT</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Xuất thông tin cơ bản và chi tiết</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t>BẢNG KẾ HOẠCH THỰC HIỆN TIỂU LUẬN CHUYÊN NGÀNH - 2019</t>
@@ -121,6 +118,39 @@
   </si>
   <si>
     <t>thiết kế các page</t>
+  </si>
+  <si>
+    <t>Cài đặt NodeJS</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về NodeJS</t>
+  </si>
+  <si>
+    <t>Tạo server-side đơn giản với NodeJS</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về MongoDB</t>
+  </si>
+  <si>
+    <t>MongoDB là gì?</t>
+  </si>
+  <si>
+    <t>NodeJS là gì?</t>
+  </si>
+  <si>
+    <t>Sử dụng Cloud MongoDB để lưu dữ liệu</t>
+  </si>
+  <si>
+    <t>Tạo connection giữa MongoDB và NodeJS</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về ReactJS</t>
+  </si>
+  <si>
+    <t>ReactJS là gì?</t>
+  </si>
+  <si>
+    <t>Tạo client-side đơn giản với ReactJS</t>
   </si>
 </sst>
 </file>
@@ -646,7 +676,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A2:J25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A2:J37">
   <tableColumns count="10">
     <tableColumn id="1" name="STT"/>
     <tableColumn id="2" name="DANH SÁCH CÔNG VIỆC"/>
@@ -960,13 +990,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Y1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -982,7 +1012,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="33.75" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1009,7 +1039,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="42.75" customHeight="1">
+    <row r="2" spans="1:25" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1020,10 +1050,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -1056,12 +1086,12 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="19.5" customHeight="1">
+    <row r="3" spans="1:25" ht="19.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
@@ -1087,26 +1117,24 @@
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
     </row>
-    <row r="4" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A4" s="14">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:25" ht="20.25" customHeight="1" thickTop="1">
+      <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="34"/>
       <c r="J4" s="36"/>
@@ -1126,29 +1154,27 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
     </row>
-    <row r="5" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A5" s="18">
-        <v>3</v>
+    <row r="5" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16" t="s">
+        <v>33</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="19" t="s">
-        <v>17</v>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>14</v>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="37" t="s">
-        <v>28</v>
+      <c r="F5" s="10"/>
+      <c r="G5" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="36"/>
       <c r="K5" s="11"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -1160,36 +1186,32 @@
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-    </row>
-    <row r="6" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A6" s="18">
-        <v>4</v>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+    </row>
+    <row r="6" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="19" t="s">
-        <v>18</v>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>14</v>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>29</v>
+      <c r="F6" s="10"/>
+      <c r="G6" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="36"/>
       <c r="K6" s="11"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -1201,26 +1223,24 @@
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A7" s="14">
-        <v>5</v>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+    </row>
+    <row r="7" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
+        <v>36</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="37"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="36"/>
       <c r="K7" s="11"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
@@ -1237,21 +1257,27 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A8" s="14">
-        <v>6</v>
+    <row r="8" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>37</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>21</v>
+      <c r="D8" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="34"/>
+      <c r="J8" s="36"/>
       <c r="K8" s="11"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
@@ -1268,23 +1294,27 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A9" s="18">
-        <v>7</v>
+    <row r="9" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
+        <v>39</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="19" t="s">
-        <v>22</v>
+      <c r="D9" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="21" t="s">
-        <v>9</v>
+      <c r="E9" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="34"/>
+      <c r="J9" s="36"/>
       <c r="K9" s="11"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
@@ -1296,26 +1326,32 @@
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-    </row>
-    <row r="10" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A10" s="18">
-        <v>8</v>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+    </row>
+    <row r="10" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16" t="s">
+        <v>40</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
-        <v>23</v>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="11"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
@@ -1327,26 +1363,24 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-    </row>
-    <row r="11" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A11" s="25">
-        <v>9</v>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+    </row>
+    <row r="11" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>41</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="11"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1358,24 +1392,32 @@
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-    </row>
-    <row r="12" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A12" s="18">
-        <v>10</v>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+    </row>
+    <row r="12" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16" t="s">
+        <v>42</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="36"/>
       <c r="K12" s="11"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -1387,26 +1429,32 @@
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-    </row>
-    <row r="13" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A13" s="18">
-        <v>11</v>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+    </row>
+    <row r="13" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16" t="s">
+        <v>43</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>25</v>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+      <c r="E13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="11"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -1418,26 +1466,22 @@
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-    </row>
-    <row r="14" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A14" s="25">
-        <v>12</v>
-      </c>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+    </row>
+    <row r="14" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="36"/>
       <c r="K14" s="11"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -1449,26 +1493,24 @@
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-    </row>
-    <row r="15" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A15" s="25">
-        <v>13</v>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+    </row>
+    <row r="15" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>14</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="36"/>
       <c r="K15" s="11"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
@@ -1480,24 +1522,32 @@
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-    </row>
-    <row r="16" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A16" s="18">
-        <v>14</v>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16" t="s">
+        <v>15</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="38"/>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="11"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
@@ -1509,24 +1559,30 @@
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-    </row>
-    <row r="17" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A17" s="14">
-        <v>15</v>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+    </row>
+    <row r="17" spans="1:25" ht="20.25" customHeight="1">
+      <c r="A17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="19" t="s">
+        <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>31</v>
+      <c r="D17" s="20" t="s">
+        <v>13</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>28</v>
+      </c>
       <c r="I17" s="37"/>
       <c r="J17" s="38"/>
       <c r="K17" s="11"/>
@@ -1540,26 +1596,32 @@
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
     </row>
     <row r="18" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A18" s="18">
-        <v>16</v>
-      </c>
+      <c r="A18" s="18"/>
       <c r="B18" s="15"/>
       <c r="C18" s="19" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="I18" s="37"/>
       <c r="J18" s="38"/>
       <c r="K18" s="11"/>
@@ -1579,20 +1641,16 @@
       <c r="Y18" s="13"/>
     </row>
     <row r="19" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A19" s="18">
-        <v>17</v>
-      </c>
+      <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="19" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="21" t="s">
-        <v>10</v>
-      </c>
+      <c r="F19" s="21"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="37"/>
       <c r="J19" s="38"/>
       <c r="K19" s="11"/>
@@ -1606,19 +1664,19 @@
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
     </row>
     <row r="20" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A20" s="25">
-        <v>18</v>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>20</v>
       </c>
-      <c r="B20" s="15"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="26"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="21"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
@@ -1635,21 +1693,21 @@
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
     </row>
     <row r="21" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A21" s="18">
-        <v>19</v>
+      <c r="A21" s="18"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="19" t="s">
+        <v>21</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
@@ -1672,16 +1730,14 @@
       <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A22" s="18">
-        <v>20</v>
+      <c r="A22" s="18"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23" t="s">
+        <v>22</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21" t="s">
-        <v>10</v>
-      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
@@ -1703,11 +1759,11 @@
       <c r="Y22" s="13"/>
     </row>
     <row r="23" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A23" s="27">
-        <v>21</v>
+      <c r="A23" s="25"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="19" t="s">
+        <v>23</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="16"/>
       <c r="D23" s="20"/>
       <c r="E23" s="26"/>
       <c r="F23" s="21"/>
@@ -1732,13 +1788,11 @@
       <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A24" s="27">
-        <v>22</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="16"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="26"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="21"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
@@ -1761,10 +1815,10 @@
       <c r="Y24" s="13"/>
     </row>
     <row r="25" spans="1:25" ht="19.5" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>11</v>
+      <c r="A25" s="18"/>
+      <c r="B25" s="15" t="s">
+        <v>24</v>
       </c>
-      <c r="B25" s="15"/>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -1789,283 +1843,349 @@
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-    </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-    </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-    </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-    </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A32" s="29"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" customHeight="1">
+    <row r="26" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+    </row>
+    <row r="27" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A27" s="25"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+    </row>
+    <row r="28" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+    </row>
+    <row r="29" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+    </row>
+    <row r="30" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A30" s="18"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+    </row>
+    <row r="31" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A31" s="18"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+    </row>
+    <row r="32" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A32" s="25"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+    </row>
+    <row r="33" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A33" s="18"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+    </row>
+    <row r="34" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A34" s="18"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+    </row>
+    <row r="35" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="13"/>
+      <c r="W35" s="13"/>
+      <c r="X35" s="13"/>
+      <c r="Y35" s="13"/>
+    </row>
+    <row r="36" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+    </row>
+    <row r="37" spans="1:25" ht="19.5" customHeight="1">
+      <c r="A37" s="18"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.75" customHeight="1">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
@@ -2088,7 +2208,7 @@
       <c r="T38" s="30"/>
       <c r="U38" s="30"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" customHeight="1">
+    <row r="39" spans="1:25" ht="15.75" customHeight="1">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="31"/>
@@ -2111,7 +2231,7 @@
       <c r="T39" s="30"/>
       <c r="U39" s="30"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" customHeight="1">
+    <row r="40" spans="1:25" ht="15.75" customHeight="1">
       <c r="A40" s="29"/>
       <c r="B40" s="30"/>
       <c r="C40" s="31"/>
@@ -2134,7 +2254,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="30"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" customHeight="1">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
@@ -2157,7 +2277,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="30"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" customHeight="1">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
@@ -2180,7 +2300,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="30"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" customHeight="1">
+    <row r="43" spans="1:25" ht="15.75" customHeight="1">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
       <c r="C43" s="31"/>
@@ -2203,7 +2323,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="30"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" customHeight="1">
+    <row r="44" spans="1:25" ht="15.75" customHeight="1">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
@@ -2226,7 +2346,7 @@
       <c r="T44" s="30"/>
       <c r="U44" s="30"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1">
       <c r="A45" s="29"/>
       <c r="B45" s="30"/>
       <c r="C45" s="31"/>
@@ -2249,7 +2369,7 @@
       <c r="T45" s="30"/>
       <c r="U45" s="30"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" customHeight="1">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="30"/>
       <c r="C46" s="31"/>
@@ -2272,7 +2392,7 @@
       <c r="T46" s="30"/>
       <c r="U46" s="30"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" customHeight="1">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1">
       <c r="A47" s="29"/>
       <c r="B47" s="30"/>
       <c r="C47" s="31"/>
@@ -2295,7 +2415,7 @@
       <c r="T47" s="30"/>
       <c r="U47" s="30"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" customHeight="1">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="30"/>
       <c r="C48" s="31"/>
@@ -24214,6 +24334,282 @@
       <c r="T1000" s="30"/>
       <c r="U1000" s="30"/>
     </row>
+    <row r="1001" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1001" s="29"/>
+      <c r="B1001" s="30"/>
+      <c r="C1001" s="31"/>
+      <c r="D1001" s="32"/>
+      <c r="E1001" s="32"/>
+      <c r="F1001" s="33"/>
+      <c r="G1001" s="41"/>
+      <c r="H1001" s="41"/>
+      <c r="I1001" s="41"/>
+      <c r="J1001" s="41"/>
+      <c r="K1001" s="30"/>
+      <c r="L1001" s="30"/>
+      <c r="M1001" s="30"/>
+      <c r="N1001" s="30"/>
+      <c r="O1001" s="30"/>
+      <c r="P1001" s="30"/>
+      <c r="Q1001" s="30"/>
+      <c r="R1001" s="30"/>
+      <c r="S1001" s="30"/>
+      <c r="T1001" s="30"/>
+      <c r="U1001" s="30"/>
+    </row>
+    <row r="1002" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1002" s="29"/>
+      <c r="B1002" s="30"/>
+      <c r="C1002" s="31"/>
+      <c r="D1002" s="32"/>
+      <c r="E1002" s="32"/>
+      <c r="F1002" s="33"/>
+      <c r="G1002" s="41"/>
+      <c r="H1002" s="41"/>
+      <c r="I1002" s="41"/>
+      <c r="J1002" s="41"/>
+      <c r="K1002" s="30"/>
+      <c r="L1002" s="30"/>
+      <c r="M1002" s="30"/>
+      <c r="N1002" s="30"/>
+      <c r="O1002" s="30"/>
+      <c r="P1002" s="30"/>
+      <c r="Q1002" s="30"/>
+      <c r="R1002" s="30"/>
+      <c r="S1002" s="30"/>
+      <c r="T1002" s="30"/>
+      <c r="U1002" s="30"/>
+    </row>
+    <row r="1003" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1003" s="29"/>
+      <c r="B1003" s="30"/>
+      <c r="C1003" s="31"/>
+      <c r="D1003" s="32"/>
+      <c r="E1003" s="32"/>
+      <c r="F1003" s="33"/>
+      <c r="G1003" s="41"/>
+      <c r="H1003" s="41"/>
+      <c r="I1003" s="41"/>
+      <c r="J1003" s="41"/>
+      <c r="K1003" s="30"/>
+      <c r="L1003" s="30"/>
+      <c r="M1003" s="30"/>
+      <c r="N1003" s="30"/>
+      <c r="O1003" s="30"/>
+      <c r="P1003" s="30"/>
+      <c r="Q1003" s="30"/>
+      <c r="R1003" s="30"/>
+      <c r="S1003" s="30"/>
+      <c r="T1003" s="30"/>
+      <c r="U1003" s="30"/>
+    </row>
+    <row r="1004" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1004" s="29"/>
+      <c r="B1004" s="30"/>
+      <c r="C1004" s="31"/>
+      <c r="D1004" s="32"/>
+      <c r="E1004" s="32"/>
+      <c r="F1004" s="33"/>
+      <c r="G1004" s="41"/>
+      <c r="H1004" s="41"/>
+      <c r="I1004" s="41"/>
+      <c r="J1004" s="41"/>
+      <c r="K1004" s="30"/>
+      <c r="L1004" s="30"/>
+      <c r="M1004" s="30"/>
+      <c r="N1004" s="30"/>
+      <c r="O1004" s="30"/>
+      <c r="P1004" s="30"/>
+      <c r="Q1004" s="30"/>
+      <c r="R1004" s="30"/>
+      <c r="S1004" s="30"/>
+      <c r="T1004" s="30"/>
+      <c r="U1004" s="30"/>
+    </row>
+    <row r="1005" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1005" s="29"/>
+      <c r="B1005" s="30"/>
+      <c r="C1005" s="31"/>
+      <c r="D1005" s="32"/>
+      <c r="E1005" s="32"/>
+      <c r="F1005" s="33"/>
+      <c r="G1005" s="41"/>
+      <c r="H1005" s="41"/>
+      <c r="I1005" s="41"/>
+      <c r="J1005" s="41"/>
+      <c r="K1005" s="30"/>
+      <c r="L1005" s="30"/>
+      <c r="M1005" s="30"/>
+      <c r="N1005" s="30"/>
+      <c r="O1005" s="30"/>
+      <c r="P1005" s="30"/>
+      <c r="Q1005" s="30"/>
+      <c r="R1005" s="30"/>
+      <c r="S1005" s="30"/>
+      <c r="T1005" s="30"/>
+      <c r="U1005" s="30"/>
+    </row>
+    <row r="1006" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1006" s="29"/>
+      <c r="B1006" s="30"/>
+      <c r="C1006" s="31"/>
+      <c r="D1006" s="32"/>
+      <c r="E1006" s="32"/>
+      <c r="F1006" s="33"/>
+      <c r="G1006" s="41"/>
+      <c r="H1006" s="41"/>
+      <c r="I1006" s="41"/>
+      <c r="J1006" s="41"/>
+      <c r="K1006" s="30"/>
+      <c r="L1006" s="30"/>
+      <c r="M1006" s="30"/>
+      <c r="N1006" s="30"/>
+      <c r="O1006" s="30"/>
+      <c r="P1006" s="30"/>
+      <c r="Q1006" s="30"/>
+      <c r="R1006" s="30"/>
+      <c r="S1006" s="30"/>
+      <c r="T1006" s="30"/>
+      <c r="U1006" s="30"/>
+    </row>
+    <row r="1007" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1007" s="29"/>
+      <c r="B1007" s="30"/>
+      <c r="C1007" s="31"/>
+      <c r="D1007" s="32"/>
+      <c r="E1007" s="32"/>
+      <c r="F1007" s="33"/>
+      <c r="G1007" s="41"/>
+      <c r="H1007" s="41"/>
+      <c r="I1007" s="41"/>
+      <c r="J1007" s="41"/>
+      <c r="K1007" s="30"/>
+      <c r="L1007" s="30"/>
+      <c r="M1007" s="30"/>
+      <c r="N1007" s="30"/>
+      <c r="O1007" s="30"/>
+      <c r="P1007" s="30"/>
+      <c r="Q1007" s="30"/>
+      <c r="R1007" s="30"/>
+      <c r="S1007" s="30"/>
+      <c r="T1007" s="30"/>
+      <c r="U1007" s="30"/>
+    </row>
+    <row r="1008" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1008" s="29"/>
+      <c r="B1008" s="30"/>
+      <c r="C1008" s="31"/>
+      <c r="D1008" s="32"/>
+      <c r="E1008" s="32"/>
+      <c r="F1008" s="33"/>
+      <c r="G1008" s="41"/>
+      <c r="H1008" s="41"/>
+      <c r="I1008" s="41"/>
+      <c r="J1008" s="41"/>
+      <c r="K1008" s="30"/>
+      <c r="L1008" s="30"/>
+      <c r="M1008" s="30"/>
+      <c r="N1008" s="30"/>
+      <c r="O1008" s="30"/>
+      <c r="P1008" s="30"/>
+      <c r="Q1008" s="30"/>
+      <c r="R1008" s="30"/>
+      <c r="S1008" s="30"/>
+      <c r="T1008" s="30"/>
+      <c r="U1008" s="30"/>
+    </row>
+    <row r="1009" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1009" s="29"/>
+      <c r="B1009" s="30"/>
+      <c r="C1009" s="31"/>
+      <c r="D1009" s="32"/>
+      <c r="E1009" s="32"/>
+      <c r="F1009" s="33"/>
+      <c r="G1009" s="41"/>
+      <c r="H1009" s="41"/>
+      <c r="I1009" s="41"/>
+      <c r="J1009" s="41"/>
+      <c r="K1009" s="30"/>
+      <c r="L1009" s="30"/>
+      <c r="M1009" s="30"/>
+      <c r="N1009" s="30"/>
+      <c r="O1009" s="30"/>
+      <c r="P1009" s="30"/>
+      <c r="Q1009" s="30"/>
+      <c r="R1009" s="30"/>
+      <c r="S1009" s="30"/>
+      <c r="T1009" s="30"/>
+      <c r="U1009" s="30"/>
+    </row>
+    <row r="1010" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1010" s="29"/>
+      <c r="B1010" s="30"/>
+      <c r="C1010" s="31"/>
+      <c r="D1010" s="32"/>
+      <c r="E1010" s="32"/>
+      <c r="F1010" s="33"/>
+      <c r="G1010" s="41"/>
+      <c r="H1010" s="41"/>
+      <c r="I1010" s="41"/>
+      <c r="J1010" s="41"/>
+      <c r="K1010" s="30"/>
+      <c r="L1010" s="30"/>
+      <c r="M1010" s="30"/>
+      <c r="N1010" s="30"/>
+      <c r="O1010" s="30"/>
+      <c r="P1010" s="30"/>
+      <c r="Q1010" s="30"/>
+      <c r="R1010" s="30"/>
+      <c r="S1010" s="30"/>
+      <c r="T1010" s="30"/>
+      <c r="U1010" s="30"/>
+    </row>
+    <row r="1011" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1011" s="29"/>
+      <c r="B1011" s="30"/>
+      <c r="C1011" s="31"/>
+      <c r="D1011" s="32"/>
+      <c r="E1011" s="32"/>
+      <c r="F1011" s="33"/>
+      <c r="G1011" s="41"/>
+      <c r="H1011" s="41"/>
+      <c r="I1011" s="41"/>
+      <c r="J1011" s="41"/>
+      <c r="K1011" s="30"/>
+      <c r="L1011" s="30"/>
+      <c r="M1011" s="30"/>
+      <c r="N1011" s="30"/>
+      <c r="O1011" s="30"/>
+      <c r="P1011" s="30"/>
+      <c r="Q1011" s="30"/>
+      <c r="R1011" s="30"/>
+      <c r="S1011" s="30"/>
+      <c r="T1011" s="30"/>
+      <c r="U1011" s="30"/>
+    </row>
+    <row r="1012" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1012" s="29"/>
+      <c r="B1012" s="30"/>
+      <c r="C1012" s="31"/>
+      <c r="D1012" s="32"/>
+      <c r="E1012" s="32"/>
+      <c r="F1012" s="33"/>
+      <c r="G1012" s="41"/>
+      <c r="H1012" s="41"/>
+      <c r="I1012" s="41"/>
+      <c r="J1012" s="41"/>
+      <c r="K1012" s="30"/>
+      <c r="L1012" s="30"/>
+      <c r="M1012" s="30"/>
+      <c r="N1012" s="30"/>
+      <c r="O1012" s="30"/>
+      <c r="P1012" s="30"/>
+      <c r="Q1012" s="30"/>
+      <c r="R1012" s="30"/>
+      <c r="S1012" s="30"/>
+      <c r="T1012" s="30"/>
+      <c r="U1012" s="30"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>